<commit_message>
finished complicated pandas example
</commit_message>
<xml_diff>
--- a/python3/pandas/cool.xlsx
+++ b/python3/pandas/cool.xlsx
@@ -454,7 +454,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -710,8 +710,8 @@
       <c r="B17" t="s">
         <v>1</v>
       </c>
-      <c r="F17" t="s">
-        <v>22</v>
+      <c r="F17" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="G17">
         <v>16</v>

</xml_diff>